<commit_message>
Added links to course list
</commit_message>
<xml_diff>
--- a/DTU_Grades.xlsx
+++ b/DTU_Grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\Fritid\Programmering\Personlig Hjemmeside\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C9E4CA-FC35-4E53-8EB6-215737F530A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6FB1D2-B145-4615-BE17-DB10137DE496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{787CE140-0CC4-449C-90A9-32B43811A6A8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Introduction to intelligent systems</t>
   </si>
@@ -106,6 +106,72 @@
   </si>
   <si>
     <t>Udvekslingsophold - Sungkyunkwan University (SKKU)</t>
+  </si>
+  <si>
+    <t>01017</t>
+  </si>
+  <si>
+    <t>02631</t>
+  </si>
+  <si>
+    <t>02461</t>
+  </si>
+  <si>
+    <t>02403</t>
+  </si>
+  <si>
+    <t>01005</t>
+  </si>
+  <si>
+    <t>02462</t>
+  </si>
+  <si>
+    <t>02464</t>
+  </si>
+  <si>
+    <t>02105</t>
+  </si>
+  <si>
+    <t>26028</t>
+  </si>
+  <si>
+    <t>02809</t>
+  </si>
+  <si>
+    <t>02445</t>
+  </si>
+  <si>
+    <t>01035</t>
+  </si>
+  <si>
+    <t>02450</t>
+  </si>
+  <si>
+    <t>10024</t>
+  </si>
+  <si>
+    <t>34315</t>
+  </si>
+  <si>
+    <t>02463</t>
+  </si>
+  <si>
+    <t>02466</t>
+  </si>
+  <si>
+    <t>02465</t>
+  </si>
+  <si>
+    <t>42611</t>
+  </si>
+  <si>
+    <t>02182</t>
+  </si>
+  <si>
+    <t>02502</t>
+  </si>
+  <si>
+    <t>02170</t>
   </si>
 </sst>
 </file>
@@ -149,12 +215,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8A2871-EF50-44EF-990E-763EA4E255F7}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,10 +547,10 @@
     <col min="1" max="1" width="58.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="5" max="5" width="9" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -496,8 +563,11 @@
       <c r="D1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -510,8 +580,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -524,8 +597,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -538,8 +614,11 @@
       <c r="D4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -552,8 +631,11 @@
       <c r="D5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -566,8 +648,11 @@
       <c r="D6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -580,8 +665,11 @@
       <c r="D7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -594,8 +682,11 @@
       <c r="D8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -608,8 +699,11 @@
       <c r="D9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -622,8 +716,11 @@
       <c r="D10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -636,8 +733,11 @@
       <c r="D11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -650,8 +750,11 @@
       <c r="D12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -664,8 +767,11 @@
       <c r="D13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -678,8 +784,11 @@
       <c r="D14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -692,8 +801,11 @@
       <c r="D15">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -706,8 +818,11 @@
       <c r="D16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -720,8 +835,11 @@
       <c r="D17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -734,8 +852,11 @@
       <c r="D18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -748,8 +869,11 @@
       <c r="D19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -763,7 +887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -776,8 +900,11 @@
       <c r="D21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -790,8 +917,11 @@
       <c r="D22">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -804,8 +934,11 @@
       <c r="D23">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
     </row>
   </sheetData>

</xml_diff>